<commit_message>
adjust max weight on Real Estate in basic_asset_classes
</commit_message>
<xml_diff>
--- a/data/basic_asset_classes_constrained.xlsx
+++ b/data/basic_asset_classes_constrained.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/Desktop/Test Portfolios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D092CEE2-9ED0-49EF-A28B-1F877F7B8197}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4789503-2B0D-4BF6-9B5A-874FAFDF42D6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,6 +150,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,7 +447,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated basic asset classes to add EEM and replace IYR with GLD
</commit_message>
<xml_diff>
--- a/data/basic_asset_classes_constrained.xlsx
+++ b/data/basic_asset_classes_constrained.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4789503-2B0D-4BF6-9B5A-874FAFDF42D6}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B0BC7A-3571-4CF0-AC11-AA2124924124}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Ticker</t>
   </si>
@@ -53,9 +53,6 @@
     <t>IWM</t>
   </si>
   <si>
-    <t>IYR</t>
-  </si>
-  <si>
     <t>Curr Weight</t>
   </si>
   <si>
@@ -63,6 +60,12 @@
   </si>
   <si>
     <t>IVV</t>
+  </si>
+  <si>
+    <t>EEM</t>
+  </si>
+  <si>
+    <t>GLD</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -133,6 +136,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -150,10 +156,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,10 +446,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -496,7 +498,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -518,7 +520,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -528,13 +530,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update constraints on basic_asset_classes_constrained
</commit_message>
<xml_diff>
--- a/data/basic_asset_classes_constrained.xlsx
+++ b/data/basic_asset_classes_constrained.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B0BC7A-3571-4CF0-AC11-AA2124924124}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B0A7816-48B9-4494-B35C-12E9F0A930A5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,9 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,6 +153,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,7 +450,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>0.75</v>
+        <v>0.99999000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -504,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>0.6</v>
+        <v>0.99999000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -530,7 +531,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">

</xml_diff>

<commit_message>
revised constraints on basic asset classes portfolio
</commit_message>
<xml_diff>
--- a/data/basic_asset_classes_constrained.xlsx
+++ b/data/basic_asset_classes_constrained.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B0A7816-48B9-4494-B35C-12E9F0A930A5}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3A9D9B2-AFFA-450C-A7C8-172D2D497019}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,10 +153,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,7 +446,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>0.99999000000000005</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -505,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>0.99999000000000005</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -527,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -538,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>